<commit_message>
bj: update some forms
</commit_message>
<xml_diff>
--- a/SCH-STH/Impact assessments/Benin/2024/Oct 2024/bj_sch_sth_impact_2410_1_school.xlsx
+++ b/SCH-STH/Impact assessments/Benin/2024/Oct 2024/bj_sch_sth_impact_2410_1_school.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\SCH-STH\Impact assessments\Benin\2024\Oct 2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94971828-2F79-4B6E-A641-03839EB74FAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D315E2C9-CAF6-41BF-84F1-2A478AC96A88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -1876,12 +1876,6 @@
     <t>EPP MISSINKO/A</t>
   </si>
   <si>
-    <t>bj_sch_sth_impact_2410_1_school_v2</t>
-  </si>
-  <si>
-    <t>(2024 Octobre) - 1. SCH/STH – Ecole/Localité V2</t>
-  </si>
-  <si>
     <t>NOTRE DAME DE L.IMMACULEE</t>
   </si>
   <si>
@@ -1889,6 +1883,12 @@
   </si>
   <si>
     <t>L.AIGLE DES COLLINES</t>
+  </si>
+  <si>
+    <t>bj_sch_sth_impact_2410_1_school_v2_2</t>
+  </si>
+  <si>
+    <t>(2024 Octobre) - 1. SCH/STH – Ecole/Localité V2.2</t>
   </si>
 </sst>
 </file>
@@ -2160,17 +2160,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2542,7 +2532,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -6625,10 +6615,10 @@
         <v>143</v>
       </c>
       <c r="B225" s="5" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C225" s="5" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="F225" t="s">
         <v>384</v>
@@ -6919,10 +6909,10 @@
         <v>143</v>
       </c>
       <c r="B246" s="5" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C246" s="5" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="F246" t="s">
         <v>309</v>
@@ -8641,10 +8631,10 @@
         <v>143</v>
       </c>
       <c r="B369" s="5" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="C369" s="5" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="F369" t="s">
         <v>290</v>
@@ -11433,7 +11423,7 @@
         <v>279</v>
       </c>
       <c r="G569" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="570" spans="1:7" x14ac:dyDescent="0.25">
@@ -11531,7 +11521,7 @@
         <v>286</v>
       </c>
       <c r="G576" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="577" spans="1:7" x14ac:dyDescent="0.25">
@@ -11867,7 +11857,7 @@
         <v>310</v>
       </c>
       <c r="G600" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="601" spans="1:7" x14ac:dyDescent="0.25">
@@ -12295,10 +12285,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
-        <v>554</v>
+        <v>557</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>553</v>
+        <v>556</v>
       </c>
       <c r="C2" t="s">
         <v>214</v>
@@ -12314,7 +12304,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Q238"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="E98" sqref="E98"/>
     </sheetView>
   </sheetViews>
@@ -14589,7 +14579,7 @@
         <v>384</v>
       </c>
       <c r="Q73" s="34" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.25">
@@ -15116,7 +15106,7 @@
         <v>309</v>
       </c>
       <c r="Q94" s="34" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.25">
@@ -17065,7 +17055,7 @@
         <v>290</v>
       </c>
       <c r="E179" s="34" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="P179" s="34" t="s">
         <v>381</v>
@@ -17226,7 +17216,7 @@
         <v>309</v>
       </c>
       <c r="E186" s="34" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="P186" s="34" t="s">
         <v>449</v>
@@ -17778,7 +17768,7 @@
         <v>384</v>
       </c>
       <c r="E210" s="34" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="P210" s="34" t="s">
         <v>346</v>
@@ -17945,7 +17935,7 @@
         <v>290</v>
       </c>
       <c r="Q217" s="34" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="218" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>